<commit_message>
Converted seed data to json. Added clearing of events database
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\Database Seeds\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\Git Repos\LiveMongoDBSeeder\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
   <si>
     <t>test 1</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>categories_array</t>
+  </si>
+  <si>
+    <t>_id</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269a4</t>
   </si>
 </sst>
 </file>
@@ -498,35 +504,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -534,7 +547,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -542,7 +555,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -550,7 +563,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -558,7 +571,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -566,7 +579,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -574,7 +587,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -582,7 +595,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -590,7 +603,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -598,7 +611,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -606,7 +619,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -614,7 +627,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -622,7 +635,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -630,7 +643,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Modified seed to use json file instead and added extra fields for events
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="102">
   <si>
     <t>test 1</t>
   </si>
@@ -153,6 +153,183 @@
   </si>
   <si>
     <t>5a847edee5847831acb269a4</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269a5</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269a6</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269a7</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269a8</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269a9</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269aa</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269ab</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269ac</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269ad</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269ae</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269af</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269b0</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269b1</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269b2</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269b3</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269b4</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269b5</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269b6</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269b7</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269b8</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269b9</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269ba</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269bb</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269bc</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269bd</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269be</t>
+  </si>
+  <si>
+    <t>5a847edee5847831acb269bf</t>
+  </si>
+  <si>
+    <t>numPeople</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>startTime</t>
+  </si>
+  <si>
+    <t>endTime</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>eventOwner</t>
+  </si>
+  <si>
+    <t>Dhruuv Khurana</t>
+  </si>
+  <si>
+    <t>Nathan Diamond</t>
+  </si>
+  <si>
+    <t>Josh Stuve</t>
+  </si>
+  <si>
+    <t>Chris Vasquez</t>
+  </si>
+  <si>
+    <t>Shashi Sastry</t>
+  </si>
+  <si>
+    <t>Random descriptoin</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>goodbye</t>
+  </si>
+  <si>
+    <t>schism</t>
+  </si>
+  <si>
+    <t>polaris</t>
+  </si>
+  <si>
+    <t>architects</t>
+  </si>
+  <si>
+    <t>wage war</t>
+  </si>
+  <si>
+    <t>tool</t>
+  </si>
+  <si>
+    <t>the contortionist</t>
+  </si>
+  <si>
+    <t>polyphia</t>
+  </si>
+  <si>
+    <t>nothing</t>
+  </si>
+  <si>
+    <t>more</t>
+  </si>
+  <si>
+    <t>movements</t>
+  </si>
+  <si>
+    <t>we are here</t>
+  </si>
+  <si>
+    <t>the plot in you</t>
+  </si>
+  <si>
+    <t>fit for a king</t>
+  </si>
+  <si>
+    <t>oceans ate alaska</t>
+  </si>
+  <si>
+    <t>I cant spell</t>
+  </si>
+  <si>
+    <t>come join</t>
+  </si>
+  <si>
+    <t>time, the valuator</t>
+  </si>
+  <si>
+    <t>remember</t>
   </si>
 </sst>
 </file>
@@ -504,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,9 +692,12 @@
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -527,8 +707,26 @@
       <c r="C1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -538,224 +736,558 @@
       <c r="C2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>84</v>
+      </c>
+      <c r="I5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>86</v>
+      </c>
+      <c r="I7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>82</v>
+      </c>
+      <c r="I9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>87</v>
+      </c>
+      <c r="I10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="H11" t="s">
+        <v>83</v>
+      </c>
+      <c r="I11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="H12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="H13" t="s">
+        <v>88</v>
+      </c>
+      <c r="I13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14">
+        <v>7</v>
+      </c>
+      <c r="H14" t="s">
+        <v>89</v>
+      </c>
+      <c r="I14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="H15" t="s">
+        <v>90</v>
+      </c>
+      <c r="I15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16">
+        <v>11</v>
+      </c>
+      <c r="H16" t="s">
+        <v>91</v>
+      </c>
+      <c r="I16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+      <c r="H17" t="s">
+        <v>92</v>
+      </c>
+      <c r="I17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="H18" t="s">
+        <v>93</v>
+      </c>
+      <c r="I18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>94</v>
+      </c>
+      <c r="I19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="H20" t="s">
+        <v>95</v>
+      </c>
+      <c r="I20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="H21" t="s">
+        <v>96</v>
+      </c>
+      <c r="I21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+      <c r="H22" t="s">
+        <v>97</v>
+      </c>
+      <c r="I22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+      <c r="H23" t="s">
+        <v>81</v>
+      </c>
+      <c r="I23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="H24" t="s">
+        <v>98</v>
+      </c>
+      <c r="I24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
+      </c>
+      <c r="H25" t="s">
+        <v>99</v>
+      </c>
+      <c r="I25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
+      <c r="H26" t="s">
+        <v>100</v>
+      </c>
+      <c r="I26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27">
+        <v>6</v>
+      </c>
+      <c r="H27" t="s">
+        <v>101</v>
+      </c>
+      <c r="I27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="H28" t="s">
+        <v>83</v>
+      </c>
+      <c r="I28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>29</v>
       </c>
+      <c r="C29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="H29" t="s">
+        <v>82</v>
+      </c>
+      <c r="I29" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Generalized convert_to_json Added the user json and excel
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -683,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added rake file to use in TeamCity
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
@@ -684,7 +684,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>